<commit_message>
More black box tests
</commit_message>
<xml_diff>
--- a/Testing/BlackBoxTesting.xlsx
+++ b/Testing/BlackBoxTesting.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="142">
   <si>
     <t>Test</t>
   </si>
@@ -496,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -515,14 +515,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,12 +850,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -869,12 +872,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1224,264 +1227,330 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>81</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="9" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="9" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="9" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>141</v>
+      </c>
+      <c r="D53" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>